<commit_message>
added genre mapping into Play.R
</commit_message>
<xml_diff>
--- a/Genre_Analysis.xlsx
+++ b/Genre_Analysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kaggle\2017-12-24 - Recruit Restaurant Visitors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kaggle\2017-12-24 - Recruit Restaurant Visitors\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="air_genres" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="hpg x air" sheetId="4" r:id="rId4"/>
     <sheet name="lookup_table" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="47">
   <si>
     <t>Var1</t>
   </si>
@@ -104,13 +104,73 @@
   </si>
   <si>
     <t>Propose to map to</t>
+  </si>
+  <si>
+    <t>Bistro</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Pasta/Pizza</t>
+  </si>
+  <si>
+    <t>Shabu-shabu/Sukiyaki</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>Udon/Soba</t>
+  </si>
+  <si>
+    <t>Cantonese food</t>
+  </si>
+  <si>
+    <t>Chinese general</t>
+  </si>
+  <si>
+    <t>Dim Sum/Dumplings</t>
+  </si>
+  <si>
+    <t>Korean cuisine</t>
+  </si>
+  <si>
+    <t>Shanghai food</t>
+  </si>
+  <si>
+    <t>Sichuan food</t>
+  </si>
+  <si>
+    <t>Spain/Mediterranean cuisine</t>
+  </si>
+  <si>
+    <t>Taiwanese/Hong Kong cuisine</t>
+  </si>
+  <si>
+    <t>Thai/Vietnamese food</t>
+  </si>
+  <si>
+    <t>Manual addition, not found in the joint data</t>
+  </si>
+  <si>
+    <t>Mapped value not in air list</t>
+  </si>
+  <si>
+    <t>Thai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,8 +314,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +501,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -596,7 +670,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -606,6 +680,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -653,6 +731,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -930,7 +1013,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,6 +1142,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
@@ -1810,7 +1896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K2" sqref="K2:K17"/>
     </sheetView>
@@ -2433,16 +2519,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="28.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="29.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2701,7 +2788,380 @@
         <v>"Western food",</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" ref="C17:C34" si="1">""""&amp;A17&amp;""","</f>
+        <v>"Bar/Cocktail",</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f t="shared" ref="D17:D34" si="2">""""&amp;B17&amp;""","</f>
+        <v>"Bar/Cocktail",</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Bistro",</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Italian/French",</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Cantonese food",</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Chinese general",</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Dim Sum/Dumplings",</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"French",</v>
+      </c>
+      <c r="D22" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Italian/French",</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Korean cuisine",</v>
+      </c>
+      <c r="D23" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Yakiniku/Korean food",</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Pasta/Pizza",</v>
+      </c>
+      <c r="D24" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Italian/French",</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Shabu-shabu/Sukiyaki",</v>
+      </c>
+      <c r="D25" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Japanese food",</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Shanghai food",</v>
+      </c>
+      <c r="D26" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Sichuan food",</v>
+      </c>
+      <c r="D27" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Spain/Mediterranean cuisine",</v>
+      </c>
+      <c r="D28" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Italian/French",</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Sushi",</v>
+      </c>
+      <c r="D29" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Japanese food",</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Sweets",</v>
+      </c>
+      <c r="D30" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Sweets",</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Taiwanese/Hong Kong cuisine",</v>
+      </c>
+      <c r="D31" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Chinese",</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Thai/Vietnamese food",</v>
+      </c>
+      <c r="D32" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Thai",</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Udon/Soba",</v>
+      </c>
+      <c r="D33" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Japanese food",</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>"Western food",</v>
+      </c>
+      <c r="D34" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>"Western food",</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>